<commit_message>
added swaption helper support
</commit_message>
<xml_diff>
--- a/workbooks/hexadecimal converter.xlsx
+++ b/workbooks/hexadecimal converter.xlsx
@@ -32,58 +32,58 @@
     <t xml:space="preserve">            TempStrNoSize("\x00"""),</t>
   </si>
   <si>
-    <t xml:space="preserve">            TempStrNoSize("\x16""CALENDRIER.GAP.FINANCE"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x36""Date de départ,Période,Calendrier,Convention,Règle EOM"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x19""xlObjectTools - Calendar"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x7B""Cette fonction calcule la date relative à une date de départ, d'une période, d'un calendrier et d'une convention de calcul."),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x11""La date de départ"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x2E""L'identifiant de la période (O/N, 1W, 3M, etc)"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x0D""Le calendrier"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x1F""La convention de fin de période"),</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            TempStrNoSize("\x27""La règle d'ajustement de fin de mois   ")) ;</t>
-  </si>
-  <si>
-    <t>CALENDAR.GAP</t>
-  </si>
-  <si>
-    <t>start date,period,calendar,convention,EOM rule</t>
-  </si>
-  <si>
-    <t>xlObjectTools - Calendar</t>
-  </si>
-  <si>
-    <t>This function returns the date corresponding to the gap provided</t>
-  </si>
-  <si>
-    <t>The start date</t>
-  </si>
-  <si>
-    <t>Period identifier (O/N, 1W, etc)</t>
-  </si>
-  <si>
-    <t>Reference Calendar</t>
-  </si>
-  <si>
-    <t>End of period adjustement convention</t>
-  </si>
-  <si>
-    <t>End-of-month rule</t>
+    <t xml:space="preserve">            TempStrNoSize("\x13""COURBE.TAUX.FORWARD"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x31""Identifiant de la courbe,t1,t2,convention,trigger"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x1C""xlObjectTools - Yield Curve"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x3B""Cette fonction extrait le taux forward de la courbe pointée"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x11""Object Identifer"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x2A""La date de positionnement de l'observation"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x26""La date de terminaison du taux forward"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x29""L'indentifiant de la convention de calcul"),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            TempStrNoSize("\x17""Déclenche le recalcul  "));</t>
+  </si>
+  <si>
+    <t>CURVE.FORWARD.RATE</t>
+  </si>
+  <si>
+    <t>curve identifier,time 1,time 2,convention,trigger</t>
+  </si>
+  <si>
+    <t>xlObjectTools - Yield Curve</t>
+  </si>
+  <si>
+    <t>This function computes the forward rate for the corresponding dates</t>
+  </si>
+  <si>
+    <t>Curve identifier</t>
+  </si>
+  <si>
+    <t>The forward date</t>
+  </si>
+  <si>
+    <t>The maturity date</t>
+  </si>
+  <si>
+    <t>The identifier of the convention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigger for recalculation  </t>
   </si>
 </sst>
 </file>
@@ -415,14 +415,14 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>DEC2HEX(LEN(B1))</f>
-        <v>C</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="str">
         <f>" TempStrNoSize("&amp;""""&amp;"\x"&amp;IF(HEX2DEC(A1)&lt;16,"0","")&amp;A1&amp;""""&amp;""""&amp;B1&amp;""""&amp;"),"</f>
-        <v xml:space="preserve"> TempStrNoSize("\x0C""CALENDAR.GAP"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x12""CURVE.FORWARD.RATE"),</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -431,14 +431,14 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A21" si="0">DEC2HEX(LEN(B2))</f>
-        <v>2E</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C16" si="1">" TempStrNoSize("&amp;""""&amp;"\x"&amp;IF(HEX2DEC(A2)&lt;16,"0","")&amp;A2&amp;""""&amp;""""&amp;B2&amp;""""&amp;"),"</f>
-        <v xml:space="preserve"> TempStrNoSize("\x2E""start date,period,calendar,convention,EOM rule"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x31""curve identifier,time 1,time 2,convention,trigger"),</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
@@ -463,14 +463,14 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>1B</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x18""xlObjectTools - Calendar"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x1B""xlObjectTools - Yield Curve"),</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -505,14 +505,14 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x40""This function returns the date corresponding to the gap provided"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x43""This function computes the forward rate for the corresponding dates"),</v>
       </c>
       <c r="H7" t="s">
         <v>5</v>
@@ -521,14 +521,14 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>E</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x0E""The start date"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x10""Curve identifier"),</v>
       </c>
       <c r="H8" t="s">
         <v>6</v>
@@ -537,14 +537,14 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x20""Period identifier (O/N, 1W, etc)"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x10""The forward date"),</v>
       </c>
       <c r="H9" t="s">
         <v>7</v>
@@ -553,14 +553,14 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x12""Reference Calendar"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x11""The maturity date"),</v>
       </c>
       <c r="H10" t="s">
         <v>8</v>
@@ -569,14 +569,14 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x24""End of period adjustement convention"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x20""The identifier of the convention"),</v>
       </c>
       <c r="H11" t="s">
         <v>9</v>
@@ -585,14 +585,14 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>1B</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve"> TempStrNoSize("\x11""End-of-month rule"),</v>
+        <v xml:space="preserve"> TempStrNoSize("\x1B""Trigger for recalculation  "),</v>
       </c>
       <c r="H12" t="s">
         <v>10</v>

</xml_diff>